<commit_message>
Read bus data from input and create a power flow module.
Move power flow methods (read_bus_data and create_admittance_matrix) to the power_flow module. Add two sample files based on the two- and three-bus systems from class.
</commit_message>
<xml_diff>
--- a/data/Data.xlsx
+++ b/data/Data.xlsx
@@ -5,18 +5,16 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\kjiwa\PycharmProjects\ee454-power-system-analysis\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\kjiwa\PycharmProjects\ee454-power-system-analysis\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3E1E9866-BDA4-48C3-A877-1401076E493A}" xr6:coauthVersionLast="38" xr6:coauthVersionMax="38" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5EB8148D-5785-4B0A-A794-22B0484D3B4D}" xr6:coauthVersionLast="38" xr6:coauthVersionMax="38" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12225" xr2:uid="{96A0262C-C381-4208-80FC-9B658C6113A4}"/>
   </bookViews>
   <sheets>
-    <sheet name="Load bus data" sheetId="1" r:id="rId1"/>
-    <sheet name="Generator bus data" sheetId="2" r:id="rId2"/>
-    <sheet name="Reference voltages" sheetId="3" r:id="rId3"/>
-    <sheet name="Line data" sheetId="4" r:id="rId4"/>
+    <sheet name="Bus data" sheetId="1" r:id="rId1"/>
+    <sheet name="Line data" sheetId="4" r:id="rId2"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -28,36 +26,39 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="10">
-  <si>
-    <t>Rtotal (pu)</t>
-  </si>
-  <si>
-    <t>Xtotal (pu)</t>
-  </si>
-  <si>
-    <t>Btotal (pu)</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="11">
   <si>
     <t>Fmax (MVA)</t>
   </si>
   <si>
-    <t>Bus #</t>
-  </si>
-  <si>
-    <t>Vreference (pu)</t>
-  </si>
-  <si>
-    <t>P (MW)</t>
-  </si>
-  <si>
-    <t>Q (Mvar)</t>
-  </si>
-  <si>
     <t>Destination Bus</t>
   </si>
   <si>
     <t>Source Bus</t>
+  </si>
+  <si>
+    <t>Real Power Consumed (MW)</t>
+  </si>
+  <si>
+    <t>Reactive Power Consumed (Mvar)</t>
+  </si>
+  <si>
+    <t>Real Power Delivered (MW)</t>
+  </si>
+  <si>
+    <t>Reference Voltage (pu)</t>
+  </si>
+  <si>
+    <t>Total Resistance (pu)</t>
+  </si>
+  <si>
+    <t>Total Reactance (pu)</t>
+  </si>
+  <si>
+    <t>Total Susceptance (pu)</t>
+  </si>
+  <si>
+    <t>Bus</t>
   </si>
 </sst>
 </file>
@@ -410,142 +411,180 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5C6706C7-AE82-43C4-AF8E-576A594A4AD0}">
-  <dimension ref="A1:C12"/>
+  <dimension ref="A1:E13"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
+        <v>10</v>
+      </c>
+      <c r="B1" t="s">
+        <v>3</v>
+      </c>
+      <c r="C1" t="s">
         <v>4</v>
       </c>
-      <c r="B1" t="s">
+      <c r="D1" t="s">
+        <v>5</v>
+      </c>
+      <c r="E1" t="s">
         <v>6</v>
       </c>
-      <c r="C1" t="s">
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A2">
+        <v>1</v>
+      </c>
+      <c r="E2">
+        <v>1.05</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A3">
+        <v>2</v>
+      </c>
+      <c r="B3">
+        <v>21.7</v>
+      </c>
+      <c r="C3">
+        <v>12.7</v>
+      </c>
+      <c r="D3">
+        <v>40</v>
+      </c>
+      <c r="E3">
+        <v>1.0449999999999999</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A4">
+        <v>3</v>
+      </c>
+      <c r="B4">
+        <v>94.2</v>
+      </c>
+      <c r="C4">
+        <v>19</v>
+      </c>
+      <c r="D4">
+        <v>26</v>
+      </c>
+      <c r="E4">
+        <v>1.01</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A5">
+        <v>4</v>
+      </c>
+      <c r="B5">
+        <v>47.8</v>
+      </c>
+      <c r="C5">
+        <v>-3.9</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A6">
+        <v>5</v>
+      </c>
+      <c r="B6">
+        <v>7.6</v>
+      </c>
+      <c r="C6">
+        <v>1.6</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A7">
+        <v>6</v>
+      </c>
+      <c r="B7">
+        <v>11.2</v>
+      </c>
+      <c r="C7">
+        <v>7.5</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A8">
         <v>7</v>
       </c>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A2">
-        <v>2</v>
-      </c>
-      <c r="B2">
-        <v>21.7</v>
-      </c>
-      <c r="C2">
-        <v>12.7</v>
-      </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A3">
-        <v>3</v>
-      </c>
-      <c r="B3">
-        <v>94.2</v>
-      </c>
-      <c r="C3">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A4">
-        <v>4</v>
-      </c>
-      <c r="B4">
-        <v>47.8</v>
-      </c>
-      <c r="C4">
-        <v>-3.9</v>
-      </c>
-    </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A5">
+      <c r="B8">
+        <v>29.5</v>
+      </c>
+      <c r="C8">
+        <v>16.600000000000001</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A9">
+        <v>8</v>
+      </c>
+      <c r="B9">
+        <v>9</v>
+      </c>
+      <c r="C9">
+        <v>5.8</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A10">
+        <v>9</v>
+      </c>
+      <c r="B10">
+        <v>3.5</v>
+      </c>
+      <c r="C10">
+        <v>1.8</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A11">
+        <v>10</v>
+      </c>
+      <c r="B11">
+        <v>6.1</v>
+      </c>
+      <c r="C11">
+        <v>1.6</v>
+      </c>
+      <c r="D11">
+        <v>28</v>
+      </c>
+      <c r="E11">
+        <v>1.05</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A12">
+        <v>11</v>
+      </c>
+      <c r="B12">
+        <v>13.5</v>
+      </c>
+      <c r="C12">
+        <v>5.8</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A13">
+        <v>12</v>
+      </c>
+      <c r="B13">
+        <v>14.9</v>
+      </c>
+      <c r="C13">
         <v>5</v>
       </c>
-      <c r="B5">
-        <v>7.6</v>
-      </c>
-      <c r="C5">
-        <v>1.6</v>
-      </c>
-    </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A6">
-        <v>6</v>
-      </c>
-      <c r="B6">
-        <v>11.2</v>
-      </c>
-      <c r="C6">
-        <v>7.5</v>
-      </c>
-    </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A7">
-        <v>7</v>
-      </c>
-      <c r="B7">
-        <v>29.5</v>
-      </c>
-      <c r="C7">
-        <v>16.600000000000001</v>
-      </c>
-    </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A8">
-        <v>8</v>
-      </c>
-      <c r="B8">
-        <v>9</v>
-      </c>
-      <c r="C8">
-        <v>5.8</v>
-      </c>
-    </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A9">
-        <v>9</v>
-      </c>
-      <c r="B9">
-        <v>3.5</v>
-      </c>
-      <c r="C9">
-        <v>1.8</v>
-      </c>
-    </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A10">
-        <v>10</v>
-      </c>
-      <c r="B10">
-        <v>6.1</v>
-      </c>
-      <c r="C10">
-        <v>1.6</v>
-      </c>
-    </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A11">
-        <v>11</v>
-      </c>
-      <c r="B11">
-        <v>13.5</v>
-      </c>
-      <c r="C11">
-        <v>5.8</v>
-      </c>
-    </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A12">
-        <v>12</v>
-      </c>
-      <c r="B12">
-        <v>14.9</v>
-      </c>
-      <c r="C12">
-        <v>5</v>
+      <c r="D13">
+        <v>30</v>
+      </c>
+      <c r="E13">
+        <v>1.05</v>
       </c>
     </row>
   </sheetData>
@@ -554,125 +593,6 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C188898F-E250-40F5-8570-7F013607BA3D}">
-  <dimension ref="A1:B6"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
-        <v>4</v>
-      </c>
-      <c r="B1" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A2">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A3">
-        <v>2</v>
-      </c>
-      <c r="B3">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A4">
-        <v>3</v>
-      </c>
-      <c r="B4">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A5">
-        <v>10</v>
-      </c>
-      <c r="B5">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A6">
-        <v>12</v>
-      </c>
-      <c r="B6">
-        <v>30</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C43DBABB-0FF7-4100-A813-5B2DD797D03F}">
-  <dimension ref="A1:B6"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
-        <v>4</v>
-      </c>
-      <c r="B1" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A2">
-        <v>1</v>
-      </c>
-      <c r="B2">
-        <v>1.05</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A3">
-        <v>2</v>
-      </c>
-      <c r="B3">
-        <v>1.0449999999999999</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A4">
-        <v>3</v>
-      </c>
-      <c r="B4">
-        <v>1.01</v>
-      </c>
-    </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A5">
-        <v>10</v>
-      </c>
-      <c r="B5">
-        <v>1.05</v>
-      </c>
-    </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A6">
-        <v>12</v>
-      </c>
-      <c r="B6">
-        <v>1.05</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C31AD803-4839-4A0D-A55F-341A5B575747}">
   <dimension ref="A1:F18"/>
   <sheetViews>
@@ -682,22 +602,22 @@
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
+        <v>2</v>
+      </c>
+      <c r="B1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" t="s">
+        <v>7</v>
+      </c>
+      <c r="D1" t="s">
+        <v>8</v>
+      </c>
+      <c r="E1" t="s">
         <v>9</v>
       </c>
-      <c r="B1" t="s">
-        <v>8</v>
-      </c>
-      <c r="C1" t="s">
-        <v>0</v>
-      </c>
-      <c r="D1" t="s">
-        <v>1</v>
-      </c>
-      <c r="E1" t="s">
-        <v>2</v>
-      </c>
       <c r="F1" t="s">
-        <v>3</v>
+        <v>0</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Split the transmission line from bus 1 to 2 into two separate lines (as specified).
</commit_message>
<xml_diff>
--- a/data/Data.xlsx
+++ b/data/Data.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\kjiwa\PycharmProjects\ee454-power-system-analysis\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5EB8148D-5785-4B0A-A794-22B0484D3B4D}" xr6:coauthVersionLast="38" xr6:coauthVersionMax="38" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8A2B16CE-E10D-4D25-A74C-DE9E93763061}" xr6:coauthVersionLast="38" xr6:coauthVersionMax="38" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12225" xr2:uid="{96A0262C-C381-4208-80FC-9B658C6113A4}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12225" activeTab="1" xr2:uid="{96A0262C-C381-4208-80FC-9B658C6113A4}"/>
   </bookViews>
   <sheets>
     <sheet name="Bus data" sheetId="1" r:id="rId1"/>
@@ -413,7 +413,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5C6706C7-AE82-43C4-AF8E-576A594A4AD0}">
   <dimension ref="A1:E13"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
@@ -594,9 +594,9 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C31AD803-4839-4A0D-A55F-341A5B575747}">
-  <dimension ref="A1:F18"/>
+  <dimension ref="A1:F19"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
@@ -628,13 +628,13 @@
         <v>2</v>
       </c>
       <c r="C2">
-        <v>1.9380000000000001E-2</v>
+        <v>3.8760000000000003E-2</v>
       </c>
       <c r="D2">
-        <v>5.917E-2</v>
+        <v>0.11834</v>
       </c>
       <c r="E2">
-        <v>5.28E-2</v>
+        <v>2.64E-2</v>
       </c>
       <c r="F2">
         <v>95</v>
@@ -645,36 +645,39 @@
         <v>1</v>
       </c>
       <c r="B3">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="C3">
-        <v>5.4030000000000002E-2</v>
+        <v>3.8760000000000003E-2</v>
       </c>
       <c r="D3">
-        <v>0.22303999999999999</v>
+        <v>0.11834</v>
       </c>
       <c r="E3">
-        <v>4.9200000000000001E-2</v>
+        <v>2.64E-2</v>
       </c>
       <c r="F3">
-        <v>100</v>
+        <v>95</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" s="1">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B4">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="C4">
-        <v>4.6989999999999997E-2</v>
+        <v>5.4030000000000002E-2</v>
       </c>
       <c r="D4">
-        <v>0.19797000000000001</v>
+        <v>0.22303999999999999</v>
       </c>
       <c r="E4">
-        <v>4.3799999999999999E-2</v>
+        <v>4.9200000000000001E-2</v>
+      </c>
+      <c r="F4">
+        <v>100</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.25">
@@ -682,16 +685,16 @@
         <v>2</v>
       </c>
       <c r="B5">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="C5">
-        <v>5.8110000000000002E-2</v>
+        <v>4.6989999999999997E-2</v>
       </c>
       <c r="D5">
-        <v>0.17632</v>
+        <v>0.19797000000000001</v>
       </c>
       <c r="E5">
-        <v>3.4000000000000002E-2</v>
+        <v>4.3799999999999999E-2</v>
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.25">
@@ -699,50 +702,50 @@
         <v>2</v>
       </c>
       <c r="B6">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C6">
-        <v>5.6950000000000001E-2</v>
+        <v>5.8110000000000002E-2</v>
       </c>
       <c r="D6">
-        <v>0.17388000000000001</v>
+        <v>0.17632</v>
       </c>
       <c r="E6">
-        <v>3.4599999999999999E-2</v>
+        <v>3.4000000000000002E-2</v>
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A7" s="1">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="B7">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="C7">
-        <v>0.67010000000000003</v>
+        <v>5.6950000000000001E-2</v>
       </c>
       <c r="D7">
-        <v>0.17102999999999999</v>
+        <v>0.17388000000000001</v>
       </c>
       <c r="E7">
-        <v>1.2800000000000001E-2</v>
+        <v>3.4599999999999999E-2</v>
       </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A8" s="1">
+        <v>3</v>
+      </c>
+      <c r="B8">
         <v>4</v>
       </c>
-      <c r="B8">
-        <v>5</v>
-      </c>
       <c r="C8">
-        <v>1.3350000000000001E-2</v>
+        <v>0.67010000000000003</v>
       </c>
       <c r="D8">
-        <v>4.2110000000000002E-2</v>
+        <v>0.17102999999999999</v>
       </c>
       <c r="E8">
-        <v>0</v>
+        <v>1.2800000000000001E-2</v>
       </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.25">
@@ -750,13 +753,13 @@
         <v>4</v>
       </c>
       <c r="B9">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="C9">
-        <v>0</v>
+        <v>1.3350000000000001E-2</v>
       </c>
       <c r="D9">
-        <v>0.55618000000000001</v>
+        <v>4.2110000000000002E-2</v>
       </c>
       <c r="E9">
         <v>0</v>
@@ -764,16 +767,16 @@
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A10" s="1">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B10">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="C10">
         <v>0</v>
       </c>
       <c r="D10">
-        <v>0.25202000000000002</v>
+        <v>0.55618000000000001</v>
       </c>
       <c r="E10">
         <v>0</v>
@@ -781,16 +784,16 @@
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A11" s="1">
+        <v>5</v>
+      </c>
+      <c r="B11">
         <v>6</v>
       </c>
-      <c r="B11">
-        <v>9</v>
-      </c>
       <c r="C11">
-        <v>9.4979999999999995E-2</v>
+        <v>0</v>
       </c>
       <c r="D11">
-        <v>0.19889999999999999</v>
+        <v>0.25202000000000002</v>
       </c>
       <c r="E11">
         <v>0</v>
@@ -801,13 +804,13 @@
         <v>6</v>
       </c>
       <c r="B12">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="C12">
-        <v>0.12291000000000001</v>
+        <v>9.4979999999999995E-2</v>
       </c>
       <c r="D12">
-        <v>0.25580999999999998</v>
+        <v>0.19889999999999999</v>
       </c>
       <c r="E12">
         <v>0</v>
@@ -818,13 +821,13 @@
         <v>6</v>
       </c>
       <c r="B13">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="C13">
-        <v>6.615E-2</v>
+        <v>0.12291000000000001</v>
       </c>
       <c r="D13">
-        <v>0.13027</v>
+        <v>0.25580999999999998</v>
       </c>
       <c r="E13">
         <v>0</v>
@@ -832,16 +835,16 @@
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A14" s="1">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B14">
-        <v>8</v>
+        <v>11</v>
       </c>
       <c r="C14">
-        <v>3.1809999999999998E-2</v>
+        <v>6.615E-2</v>
       </c>
       <c r="D14">
-        <v>8.4500000000000006E-2</v>
+        <v>0.13027</v>
       </c>
       <c r="E14">
         <v>0</v>
@@ -852,13 +855,13 @@
         <v>7</v>
       </c>
       <c r="B15">
-        <v>12</v>
+        <v>8</v>
       </c>
       <c r="C15">
-        <v>0.12711</v>
+        <v>3.1809999999999998E-2</v>
       </c>
       <c r="D15">
-        <v>0.27038000000000001</v>
+        <v>8.4500000000000006E-2</v>
       </c>
       <c r="E15">
         <v>0</v>
@@ -866,16 +869,16 @@
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A16" s="1">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B16">
-        <v>9</v>
+        <v>12</v>
       </c>
       <c r="C16">
-        <v>8.2049999999999998E-2</v>
+        <v>0.12711</v>
       </c>
       <c r="D16">
-        <v>0.19206999999999999</v>
+        <v>0.27038000000000001</v>
       </c>
       <c r="E16">
         <v>0</v>
@@ -883,16 +886,16 @@
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A17" s="1">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="B17">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="C17">
-        <v>0.22092000000000001</v>
+        <v>8.2049999999999998E-2</v>
       </c>
       <c r="D17">
-        <v>0.19988</v>
+        <v>0.19206999999999999</v>
       </c>
       <c r="E17">
         <v>0</v>
@@ -900,18 +903,35 @@
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A18" s="1">
+        <v>10</v>
+      </c>
+      <c r="B18">
         <v>11</v>
       </c>
-      <c r="B18">
+      <c r="C18">
+        <v>0.22092000000000001</v>
+      </c>
+      <c r="D18">
+        <v>0.19988</v>
+      </c>
+      <c r="E18">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A19" s="1">
+        <v>11</v>
+      </c>
+      <c r="B19">
         <v>12</v>
       </c>
-      <c r="C18">
+      <c r="C19">
         <v>0.17093</v>
       </c>
-      <c r="D18">
+      <c r="D19">
         <v>0.34802</v>
       </c>
-      <c r="E18">
+      <c r="E19">
         <v>0</v>
       </c>
     </row>

</xml_diff>